<commit_message>
Análisis Descriptivo Series de tiempo
</commit_message>
<xml_diff>
--- a/R/Analisis Descriptivo Series de Tiempo/DesempleoyEmpleo.xlsx
+++ b/R/Analisis Descriptivo Series de Tiempo/DesempleoyEmpleo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A3DEC2-BFD8-3F41-94C6-BE0D85E4F14A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD31A536-C021-5148-8C20-BB2E6BA18E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1056,6 +1056,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1063,15 +1072,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1414,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D269"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="C249" sqref="C249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1423,23 +1423,23 @@
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="0.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
     <col min="5" max="6" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
@@ -4123,124 +4123,124 @@
       </c>
     </row>
     <row r="251" spans="1:4">
-      <c r="A251" s="18" t="s">
+      <c r="A251" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B251" s="18"/>
-      <c r="C251" s="18"/>
-      <c r="D251" s="18"/>
+      <c r="B251" s="21"/>
+      <c r="C251" s="21"/>
+      <c r="D251" s="21"/>
     </row>
     <row r="252" spans="1:4">
-      <c r="A252" s="18" t="s">
+      <c r="A252" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="B252" s="18"/>
-      <c r="C252" s="18"/>
-      <c r="D252" s="18"/>
+      <c r="B252" s="21"/>
+      <c r="C252" s="21"/>
+      <c r="D252" s="21"/>
     </row>
     <row r="253" spans="1:4">
-      <c r="A253" s="19" t="s">
+      <c r="A253" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="B253" s="19"/>
-      <c r="C253" s="19"/>
-      <c r="D253" s="19"/>
+      <c r="B253" s="18"/>
+      <c r="C253" s="18"/>
+      <c r="D253" s="18"/>
     </row>
     <row r="254" spans="1:4">
-      <c r="A254" s="19" t="s">
+      <c r="A254" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="B254" s="19"/>
-      <c r="C254" s="19"/>
-      <c r="D254" s="19"/>
+      <c r="B254" s="18"/>
+      <c r="C254" s="18"/>
+      <c r="D254" s="18"/>
     </row>
     <row r="255" spans="1:4">
-      <c r="A255" s="19" t="s">
+      <c r="A255" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B255" s="19"/>
-      <c r="C255" s="19"/>
-      <c r="D255" s="19"/>
+      <c r="B255" s="18"/>
+      <c r="C255" s="18"/>
+      <c r="D255" s="18"/>
     </row>
     <row r="256" spans="1:4">
-      <c r="A256" s="19" t="s">
+      <c r="A256" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="B256" s="19"/>
-      <c r="C256" s="19"/>
-      <c r="D256" s="19"/>
+      <c r="B256" s="18"/>
+      <c r="C256" s="18"/>
+      <c r="D256" s="18"/>
     </row>
     <row r="257" spans="1:4">
-      <c r="A257" s="20" t="s">
+      <c r="A257" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="B257" s="20"/>
-      <c r="C257" s="20"/>
-      <c r="D257" s="20"/>
+      <c r="B257" s="16"/>
+      <c r="C257" s="16"/>
+      <c r="D257" s="16"/>
     </row>
     <row r="258" spans="1:4">
-      <c r="A258" s="20" t="s">
+      <c r="A258" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="B258" s="20"/>
-      <c r="C258" s="20"/>
-      <c r="D258" s="20"/>
+      <c r="B258" s="16"/>
+      <c r="C258" s="16"/>
+      <c r="D258" s="16"/>
     </row>
     <row r="259" spans="1:4">
-      <c r="A259" s="20" t="s">
+      <c r="A259" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="B259" s="20"/>
-      <c r="C259" s="20"/>
-      <c r="D259" s="20"/>
+      <c r="B259" s="16"/>
+      <c r="C259" s="16"/>
+      <c r="D259" s="16"/>
     </row>
     <row r="260" spans="1:4">
-      <c r="A260" s="20" t="s">
+      <c r="A260" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="B260" s="20"/>
-      <c r="C260" s="20"/>
-      <c r="D260" s="20"/>
+      <c r="B260" s="16"/>
+      <c r="C260" s="16"/>
+      <c r="D260" s="16"/>
     </row>
     <row r="261" spans="1:4">
-      <c r="A261" s="20" t="s">
+      <c r="A261" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="B261" s="20"/>
-      <c r="C261" s="20"/>
-      <c r="D261" s="20"/>
+      <c r="B261" s="16"/>
+      <c r="C261" s="16"/>
+      <c r="D261" s="16"/>
     </row>
     <row r="262" spans="1:4">
-      <c r="A262" s="20" t="s">
+      <c r="A262" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="B262" s="20"/>
-      <c r="C262" s="20"/>
-      <c r="D262" s="20"/>
+      <c r="B262" s="16"/>
+      <c r="C262" s="16"/>
+      <c r="D262" s="16"/>
     </row>
     <row r="263" spans="1:4">
-      <c r="A263" s="20" t="s">
+      <c r="A263" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="B263" s="20"/>
-      <c r="C263" s="20"/>
-      <c r="D263" s="20"/>
+      <c r="B263" s="16"/>
+      <c r="C263" s="16"/>
+      <c r="D263" s="16"/>
     </row>
     <row r="264" spans="1:4">
-      <c r="A264" s="20" t="s">
+      <c r="A264" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="B264" s="20"/>
-      <c r="C264" s="20"/>
-      <c r="D264" s="20"/>
+      <c r="B264" s="16"/>
+      <c r="C264" s="16"/>
+      <c r="D264" s="16"/>
     </row>
     <row r="265" spans="1:4">
-      <c r="A265" s="20" t="s">
+      <c r="A265" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="B265" s="20"/>
-      <c r="C265" s="20"/>
-      <c r="D265" s="20"/>
+      <c r="B265" s="16"/>
+      <c r="C265" s="16"/>
+      <c r="D265" s="16"/>
     </row>
     <row r="266" spans="1:4">
       <c r="A266" s="14" t="s">
@@ -4248,20 +4248,20 @@
       </c>
     </row>
     <row r="267" spans="1:4">
-      <c r="A267" s="21" t="s">
+      <c r="A267" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="B267" s="21"/>
-      <c r="C267" s="21"/>
-      <c r="D267" s="21"/>
+      <c r="B267" s="17"/>
+      <c r="C267" s="17"/>
+      <c r="D267" s="17"/>
     </row>
     <row r="268" spans="1:4">
-      <c r="A268" s="21" t="s">
+      <c r="A268" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="B268" s="21"/>
-      <c r="C268" s="21"/>
-      <c r="D268" s="21"/>
+      <c r="B268" s="17"/>
+      <c r="C268" s="17"/>
+      <c r="D268" s="17"/>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" s="15" t="s">
@@ -4270,6 +4270,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A251:D251"/>
+    <mergeCell ref="A252:D252"/>
+    <mergeCell ref="A253:D253"/>
+    <mergeCell ref="A254:D254"/>
+    <mergeCell ref="A255:D255"/>
+    <mergeCell ref="A256:D256"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="A258:D258"/>
     <mergeCell ref="A264:D264"/>
     <mergeCell ref="A265:D265"/>
     <mergeCell ref="A267:D267"/>
@@ -4279,16 +4289,6 @@
     <mergeCell ref="A261:D261"/>
     <mergeCell ref="A262:D262"/>
     <mergeCell ref="A263:D263"/>
-    <mergeCell ref="A254:D254"/>
-    <mergeCell ref="A255:D255"/>
-    <mergeCell ref="A256:D256"/>
-    <mergeCell ref="A257:D257"/>
-    <mergeCell ref="A258:D258"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A251:D251"/>
-    <mergeCell ref="A252:D252"/>
-    <mergeCell ref="A253:D253"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A254" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>